<commit_message>
Add validation in RuleEngineController and update template
Enhanced RuleEngineController.cs to include checks for null or
whitespace field names and non-existent properties in the loop
processing rule conditions. Updated Template.xlsx with unspecified
changes due to its binary format.
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milad\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milad\source\repos\RuleEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D890C6B9-ED36-4E2B-A7A3-104B3BF53472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5A1850-ECC8-4549-BDB5-CA4AB3C9CBBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{924DBF76-7FCD-4444-B85D-2824FA801479}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{924DBF76-7FCD-4444-B85D-2824FA801479}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -115,6 +115,18 @@
   </si>
   <si>
     <t>ISF</t>
+  </si>
+  <si>
+    <t>Condition_3</t>
+  </si>
+  <si>
+    <t>CabinClass</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -221,12 +233,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2F159BE1-50B9-4C5B-827A-E9DECC621E96}" name="Rules" displayName="Rules" ref="A1:E15" totalsRowShown="0">
-  <autoFilter ref="A1:E15" xr:uid="{2F159BE1-50B9-4C5B-827A-E9DECC621E96}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2F159BE1-50B9-4C5B-827A-E9DECC621E96}" name="Rules" displayName="Rules" ref="A1:F15" totalsRowShown="0">
+  <autoFilter ref="A1:F15" xr:uid="{2F159BE1-50B9-4C5B-827A-E9DECC621E96}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{373E484D-5D75-4CF6-AB17-1A7A129B1ED3}" name="Index"/>
     <tableColumn id="2" xr3:uid="{5DF3A7F3-C5E4-4E92-AA18-A06F91B863B2}" name="Condition_1"/>
     <tableColumn id="3" xr3:uid="{042F5900-8298-45CB-9B74-EE4A3591B2F0}" name="Condition_2"/>
+    <tableColumn id="6" xr3:uid="{27B8AEAD-2FBA-4991-B402-FA9B7E3E6816}" name="Condition_3"/>
     <tableColumn id="4" xr3:uid="{3D399EEF-64C3-42A2-A5FC-D916AF098AE5}" name="Action_1"/>
     <tableColumn id="5" xr3:uid="{5F071641-90A2-4A40-9470-CDC7CE70529C}" name="Action_2"/>
   </tableColumns>
@@ -556,8 +569,8 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView zoomScale="167" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,10 +639,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,12 +650,13 @@
     <col min="1" max="1" width="13.109375" customWidth="1"/>
     <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -653,13 +667,16 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -670,13 +687,16 @@
         <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -687,15 +707,18 @@
         <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
@@ -703,14 +726,17 @@
       <c r="C4" t="s">
         <v>24</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4">
         <v>3000</v>
       </c>
-      <c r="E4" t="b">
+      <c r="F4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -720,10 +746,13 @@
       <c r="C5" t="s">
         <v>25</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5">
         <v>5000</v>
       </c>
-      <c r="E5" t="b">
+      <c r="F5" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Rete algorithm for rule application
Introduced `ApplyRulesRete` endpoint in `RuleEngineController` and `ApplyRulesWithRete` method in `RuleEngineService` to handle rule application using the Rete algorithm. Added `ReteNetwork` class for managing and matching rules. Moved `EvaluateCondition` to `Rule` class and `GetRuleField` to `RuleSetDbModel` for better encapsulation. Updated `RuleEngineService` to use `ReteNetwork`. Modified `Template.xlsx` file.
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milad\source\repos\RuleEngine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milad\source\repos\Apex.RuleGrid\Apex.RuleGrid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5A1850-ECC8-4549-BDB5-CA4AB3C9CBBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC66F1DE-00F3-4473-B3EF-72345FEB2A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{924DBF76-7FCD-4444-B85D-2824FA801479}"/>
+    <workbookView xWindow="5496" yWindow="2220" windowWidth="17280" windowHeight="9960" activeTab="1" xr2:uid="{924DBF76-7FCD-4444-B85D-2824FA801479}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -569,7 +569,7 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
+    <sheetView zoomScale="167" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -641,8 +641,8 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>